<commit_message>
Update Oplossen fouten uit test 20220704.xlsx
</commit_message>
<xml_diff>
--- a/Overgangsrecht+TAM/Oplossen fouten uit test 20220704.xlsx
+++ b/Overgangsrecht+TAM/Oplossen fouten uit test 20220704.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Github\Geonovum\imro-dev\Overgangsrecht+TAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD9883E-F9FD-409A-8993-1A79BAE27951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A97BA55-9A6F-4C11-A3B8-595E4C1EA760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3B9409DF-38CF-4439-A4D2-12BFE7E549DF}"/>
   </bookViews>
@@ -804,7 +804,7 @@
   <dimension ref="A1:FC48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>